<commit_message>
Finished psych and half of orgo.
</commit_message>
<xml_diff>
--- a/MCAT Study Schedule.xlsx
+++ b/MCAT Study Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myaomeow/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myaomeow/Desktop/Caltech/SU2019/MCAT_Study_Guide_SU2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A3DE3F5-7E96-444F-8988-8D4FA945C68F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BC08FF-8D8D-CD46-97CC-3DBE93589BD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{5263220E-86DD-A44E-9684-31A1A93695C4}"/>
   </bookViews>
@@ -31,34 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Equilibrium</t>
-  </si>
-  <si>
-    <t>Titration Curves</t>
-  </si>
-  <si>
-    <t>The Biology Behind Behavior</t>
-  </si>
-  <si>
-    <t>The Human Senses</t>
-  </si>
-  <si>
-    <t>Learning and Memory</t>
-  </si>
-  <si>
-    <t>Emotion, Stress, Motivation, and Addiction</t>
-  </si>
-  <si>
-    <t>Cognition and Consciousness</t>
-  </si>
-  <si>
-    <t>Personality and Attitudes</t>
-  </si>
-  <si>
-    <t>Psychological Disorders</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Metabolic Components</t>
   </si>
@@ -67,12 +40,6 @@
   </si>
   <si>
     <t>Expression of Genetic Information</t>
-  </si>
-  <si>
-    <t>Spectroscopy</t>
-  </si>
-  <si>
-    <t>Lab Techniques</t>
   </si>
   <si>
     <t>Lipids</t>
@@ -443,7 +410,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,88 +419,55 @@
       <c r="A1" s="1">
         <v>43677</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43678</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43679</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43680</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43681</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43682</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43683</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43684</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -541,10 +475,10 @@
         <v>43685</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -552,7 +486,7 @@
         <v>43686</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished lipids for ochem.
</commit_message>
<xml_diff>
--- a/MCAT Study Schedule.xlsx
+++ b/MCAT Study Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myaomeow/Desktop/Caltech/SU2019/MCAT_Study_Guide_SU2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BC08FF-8D8D-CD46-97CC-3DBE93589BD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95CFE14-38CA-244A-84D5-4C124710EB4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{5263220E-86DD-A44E-9684-31A1A93695C4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Metabolic Components</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Expression of Genetic Information</t>
   </si>
   <si>
-    <t>Lipids</t>
-  </si>
-  <si>
     <t>Carbonyls and Alcohols</t>
   </si>
   <si>
@@ -55,6 +52,21 @@
   </si>
   <si>
     <t>CARS</t>
+  </si>
+  <si>
+    <t>Catchup</t>
+  </si>
+  <si>
+    <t>Review all notes. Print all notes.</t>
+  </si>
+  <si>
+    <t>Practice Exam 1</t>
+  </si>
+  <si>
+    <t>Practice Exam 2</t>
+  </si>
+  <si>
+    <t>Review practice exam. Do practice problems. Study flashcards.</t>
   </si>
 </sst>
 </file>
@@ -90,9 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,139 +422,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9220AABD-3BC4-AC45-B6FF-F99F33AA174A}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
-        <v>43677</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43683</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43678</v>
+        <v>43684</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43685</v>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>43679</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43680</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43686</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43681</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43687</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43682</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43688</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43683</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43689</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>43684</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43690</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43685</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43691</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>43686</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43692</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>43687</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43693</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>43688</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43694</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>43689</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43695</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>43690</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>43691</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>43692</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>43693</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>43695</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
         <v>43696</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:C12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>